<commit_message>
Changes are not reflecting on Streamlit, Thats why committing again
</commit_message>
<xml_diff>
--- a/MCUMPU_database_23_05_newest.xlsx
+++ b/MCUMPU_database_23_05_newest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://renesasgroup-my.sharepoint.com/personal/rohith_srinivasan_wr_renesas_com/Documents/Desktop/New_Workspace_25/11_03/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="16" documentId="11_11E21920B843918DAEE94763051ACF32DB84E3F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F571FB1D-555C-4941-9815-718D4EB0DBB6}"/>
+  <xr:revisionPtr revIDLastSave="32" documentId="11_11E21920B843918DAEE94763051ACF32DB84E3F4" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AF4A753B-5069-4FC7-9B42-9E6198D38DEF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19430,8 +19430,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:BO211"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="AK9" sqref="AK9"/>
+    <sheetView tabSelected="1" topLeftCell="AS1" workbookViewId="0">
+      <selection activeCell="BB2" sqref="BB2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -19444,8 +19444,20 @@
     <col min="33" max="33" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="38" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="40" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="18" bestFit="1" customWidth="1"/>
     <col min="44" max="44" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="15.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:67" x14ac:dyDescent="0.25">
@@ -19775,7 +19787,7 @@
       <c r="AO2" t="s">
         <v>106</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AP2" s="2" t="s">
         <v>107</v>
       </c>
       <c r="AQ2" t="s">
@@ -19787,7 +19799,7 @@
       <c r="AS2" t="s">
         <v>110</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AT2" s="2" t="s">
         <v>111</v>
       </c>
       <c r="AU2" t="s">
@@ -19987,7 +19999,7 @@
       <c r="AS3" t="s">
         <v>175</v>
       </c>
-      <c r="AT3" t="s">
+      <c r="AT3" s="2" t="s">
         <v>176</v>
       </c>
       <c r="AU3" t="s">
@@ -20169,7 +20181,7 @@
       <c r="AR4" t="s">
         <v>235</v>
       </c>
-      <c r="AT4" t="s">
+      <c r="AT4" s="2" t="s">
         <v>236</v>
       </c>
       <c r="AV4" t="s">
@@ -20348,7 +20360,7 @@
       <c r="AR5" t="s">
         <v>292</v>
       </c>
-      <c r="AT5" t="s">
+      <c r="AT5" s="2" t="s">
         <v>293</v>
       </c>
       <c r="AV5" t="s">
@@ -20494,7 +20506,7 @@
       <c r="AR6" t="s">
         <v>340</v>
       </c>
-      <c r="AT6" t="s">
+      <c r="AT6" s="2" t="s">
         <v>341</v>
       </c>
       <c r="AV6" t="s">
@@ -20619,7 +20631,7 @@
       <c r="AR7" t="s">
         <v>379</v>
       </c>
-      <c r="AT7" t="s">
+      <c r="AT7" s="2" t="s">
         <v>380</v>
       </c>
       <c r="AV7" t="s">
@@ -20735,7 +20747,7 @@
       <c r="AR8" t="s">
         <v>416</v>
       </c>
-      <c r="AT8" t="s">
+      <c r="AT8" s="2" t="s">
         <v>182</v>
       </c>
       <c r="AV8" t="s">
@@ -20848,7 +20860,7 @@
       <c r="AR9" t="s">
         <v>451</v>
       </c>
-      <c r="AT9" t="s">
+      <c r="AT9" s="2" t="s">
         <v>452</v>
       </c>
       <c r="AV9" t="s">
@@ -20952,7 +20964,7 @@
       <c r="AR10" t="s">
         <v>485</v>
       </c>
-      <c r="AT10" t="s">
+      <c r="AT10" s="2" t="s">
         <v>486</v>
       </c>
       <c r="AV10" t="s">
@@ -21050,7 +21062,7 @@
       <c r="AR11" t="s">
         <v>517</v>
       </c>
-      <c r="AT11" t="s">
+      <c r="AT11" s="2" t="s">
         <v>518</v>
       </c>
       <c r="AV11" t="s">
@@ -21145,7 +21157,7 @@
       <c r="AR12" t="s">
         <v>548</v>
       </c>
-      <c r="AT12" t="s">
+      <c r="AT12" s="2" t="s">
         <v>549</v>
       </c>
       <c r="AV12" t="s">
@@ -21237,7 +21249,7 @@
       <c r="AR13" t="s">
         <v>578</v>
       </c>
-      <c r="AT13" t="s">
+      <c r="AT13" s="2" t="s">
         <v>579</v>
       </c>
       <c r="AV13" t="s">
@@ -21314,7 +21326,7 @@
       <c r="AR14" t="s">
         <v>603</v>
       </c>
-      <c r="AT14" t="s">
+      <c r="AT14" s="2" t="s">
         <v>604</v>
       </c>
       <c r="AV14" t="s">
@@ -21385,7 +21397,7 @@
       <c r="AR15" t="s">
         <v>626</v>
       </c>
-      <c r="AT15" t="s">
+      <c r="AT15" s="2" t="s">
         <v>627</v>
       </c>
       <c r="AV15" t="s">
@@ -21456,7 +21468,7 @@
       <c r="AR16" t="s">
         <v>648</v>
       </c>
-      <c r="AT16" t="s">
+      <c r="AT16" s="2" t="s">
         <v>649</v>
       </c>
       <c r="AV16" t="s">
@@ -21524,7 +21536,7 @@
       <c r="AR17" t="s">
         <v>669</v>
       </c>
-      <c r="AT17" t="s">
+      <c r="AT17" s="2" t="s">
         <v>670</v>
       </c>
       <c r="AV17" t="s">
@@ -21592,7 +21604,7 @@
       <c r="AR18" t="s">
         <v>690</v>
       </c>
-      <c r="AT18" t="s">
+      <c r="AT18" s="2" t="s">
         <v>691</v>
       </c>
       <c r="AZ18" t="s">
@@ -21654,7 +21666,7 @@
       <c r="AR19" t="s">
         <v>709</v>
       </c>
-      <c r="AT19" t="s">
+      <c r="AT19" s="2" t="s">
         <v>710</v>
       </c>
       <c r="AZ19" t="s">
@@ -21713,7 +21725,7 @@
       <c r="AR20" t="s">
         <v>727</v>
       </c>
-      <c r="AT20" t="s">
+      <c r="AT20" s="2" t="s">
         <v>728</v>
       </c>
       <c r="AZ20" t="s">
@@ -21772,7 +21784,7 @@
       <c r="AR21" t="s">
         <v>745</v>
       </c>
-      <c r="AT21" t="s">
+      <c r="AT21" s="2" t="s">
         <v>746</v>
       </c>
       <c r="BD21" t="s">
@@ -21822,7 +21834,7 @@
       <c r="AR22" t="s">
         <v>759</v>
       </c>
-      <c r="AT22" t="s">
+      <c r="AT22" s="2" t="s">
         <v>760</v>
       </c>
       <c r="BD22" t="s">

</xml_diff>